<commit_message>
add a size column to the order upload in excel
</commit_message>
<xml_diff>
--- a/src/xlsx/order_with_discounts.xlsx
+++ b/src/xlsx/order_with_discounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliakendo/Documents/python/CabinetOpt/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliakendo/Documents/python/CabinetOpt/src/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F783766F-9774-594C-AF2B-DDF0BE2C5DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E8EBCC-673F-0543-B6BF-F6F18993C782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{4CF93ACF-5A75-EF4A-B0A5-918C30296281}"/>
+    <workbookView xWindow="10800" yWindow="1940" windowWidth="28240" windowHeight="17240" xr2:uid="{4CF93ACF-5A75-EF4A-B0A5-918C30296281}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Поставщик:</t>
   </si>
@@ -112,6 +111,9 @@
   </si>
   <si>
     <t>Сумма без скидки</t>
+  </si>
+  <si>
+    <t>Размер</t>
   </si>
 </sst>
 </file>
@@ -156,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -261,11 +263,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -297,6 +365,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -306,44 +413,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,7 +757,7 @@
   <dimension ref="A1:AP29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:AM7"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="11.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -693,335 +788,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:42" ht="16" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="11"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
     </row>
     <row r="2" spans="2:42" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
     </row>
     <row r="3" spans="2:42" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="25"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+      <c r="AN3" s="25"/>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
     </row>
     <row r="4" spans="2:42" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:42" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
     </row>
     <row r="6" spans="2:42" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:42" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
-      <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="14"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="14"/>
-      <c r="AM7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="15"/>
     </row>
     <row r="8" spans="2:42" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:42" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16" t="s">
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16" t="s">
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16" t="s">
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16" t="s">
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="15" t="s">
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="15"/>
-      <c r="AH9" s="15"/>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="16" t="s">
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-      <c r="AM9" s="16"/>
-      <c r="AN9" s="16"/>
+      <c r="AK9" s="17"/>
+      <c r="AL9" s="17"/>
+      <c r="AM9" s="17"/>
+      <c r="AN9" s="17"/>
       <c r="AO9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:42" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
+      <c r="B10" s="18">
         <v>0</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="20">
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="21">
         <v>0</v>
       </c>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20">
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21">
         <v>0</v>
       </c>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="20">
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="21">
         <v>0</v>
       </c>
-      <c r="AK10" s="20"/>
-      <c r="AL10" s="20"/>
-      <c r="AM10" s="20"/>
-      <c r="AN10" s="20"/>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="21"/>
+      <c r="AM10" s="21"/>
+      <c r="AN10" s="21"/>
       <c r="AO10" s="4">
         <v>0</v>
       </c>
@@ -1029,18 +1126,18 @@
     <row r="11" spans="2:42" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -1076,20 +1173,20 @@
       <c r="AD12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AE12" s="24">
+      <c r="AE12" s="12">
         <v>0</v>
       </c>
-      <c r="AF12" s="24"/>
-      <c r="AG12" s="24"/>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="25">
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="13">
         <v>0</v>
       </c>
-      <c r="AK12" s="25"/>
-      <c r="AL12" s="25"/>
-      <c r="AM12" s="25"/>
-      <c r="AN12" s="25"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="13"/>
       <c r="AO12" s="6">
         <v>0</v>
       </c>
@@ -1107,87 +1204,87 @@
       </c>
     </row>
     <row r="14" spans="2:42" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
-      <c r="AJ14" s="26"/>
-      <c r="AK14" s="26"/>
-      <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
     </row>
     <row r="15" spans="2:42" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
-      <c r="AG15" s="14"/>
-      <c r="AH15" s="14"/>
-      <c r="AI15" s="14"/>
-      <c r="AJ15" s="14"/>
-      <c r="AK15" s="14"/>
-      <c r="AL15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+      <c r="AL15" s="15"/>
     </row>
     <row r="16" spans="2:42" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -1238,34 +1335,34 @@
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
       <c r="U18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="23"/>
-      <c r="AG18" s="23"/>
-      <c r="AH18" s="23"/>
-      <c r="AI18" s="23"/>
-      <c r="AJ18" s="23"/>
-      <c r="AK18" s="23"/>
-      <c r="AL18" s="23"/>
-      <c r="AM18" s="23"/>
-      <c r="AN18" s="23"/>
-      <c r="AO18" s="23"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
     </row>
     <row r="19" spans="2:41" ht="16" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:41" ht="16" x14ac:dyDescent="0.2"/>
@@ -1278,17 +1375,20 @@
     <row r="27" spans="2:41" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="29" spans="2:41" ht="16" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="I18:R18"/>
-    <mergeCell ref="AC18:AO18"/>
-    <mergeCell ref="AE12:AI12"/>
-    <mergeCell ref="AJ12:AN12"/>
-    <mergeCell ref="B14:AM14"/>
-    <mergeCell ref="B15:AL15"/>
+  <mergeCells count="30">
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="D9:L9"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="B1:AP2"/>
+    <mergeCell ref="B3:AP3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:AM5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:AM7"/>
     <mergeCell ref="AE9:AI9"/>
     <mergeCell ref="AJ9:AN9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:O10"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="T10:V10"/>
     <mergeCell ref="W10:Y10"/>
@@ -1296,17 +1396,16 @@
     <mergeCell ref="AE10:AI10"/>
     <mergeCell ref="AJ10:AN10"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:O9"/>
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="T9:V9"/>
     <mergeCell ref="W9:Y9"/>
     <mergeCell ref="Z9:AD9"/>
-    <mergeCell ref="B1:AP2"/>
-    <mergeCell ref="B3:AP3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:AM5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:AM7"/>
+    <mergeCell ref="I18:R18"/>
+    <mergeCell ref="AC18:AO18"/>
+    <mergeCell ref="AE12:AI12"/>
+    <mergeCell ref="AJ12:AN12"/>
+    <mergeCell ref="B14:AM14"/>
+    <mergeCell ref="B15:AL15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>